<commit_message>
Completed the golden_model of the RAM
</commit_message>
<xml_diff>
--- a/verification plan/verification plan.xlsx
+++ b/verification plan/verification plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shared Folders\Uni\courses\Digital circuit\digital github codes\Done\Verification-of-SPI-Slave-with-Single-Port-RAM\verification plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shared Folders\Uni\courses\Digital circuit\digital github codes\Done\spi\Verification-of-SPI-Slave-with-Single-Port-RAM\verification plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4FA812-E263-42F1-8D4C-E7DE1B722F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7B5C98-4FE1-4DB6-9B2A-556D3330C122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{BE33C207-AC50-49BB-BEDD-1F59C983F64D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BE33C207-AC50-49BB-BEDD-1F59C983F64D}"/>
   </bookViews>
   <sheets>
     <sheet name="Verification Plan" sheetId="1" r:id="rId1"/>
@@ -751,6 +751,12 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -759,12 +765,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1113,8 +1113,8 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1169,16 +1169,16 @@
       <c r="B2" s="16">
         <v>1</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="19"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="21"/>
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:13" ht="72">
@@ -1279,16 +1279,16 @@
       <c r="B6" s="8">
         <v>2</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="21"/>
       <c r="K6" s="7"/>
       <c r="M6" s="6"/>
     </row>
@@ -1328,16 +1328,16 @@
       <c r="B8" s="8">
         <v>3</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="21"/>
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:13" ht="54">
@@ -1717,16 +1717,16 @@
       <c r="B21" s="8">
         <v>4</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="21"/>
       <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" ht="54">
@@ -1889,16 +1889,16 @@
       <c r="B27" s="8">
         <v>5</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="19"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="21"/>
       <c r="K27" s="7"/>
     </row>
     <row r="28" spans="1:11" ht="72">
@@ -1968,10 +1968,10 @@
       <c r="B30" s="1">
         <v>5.3</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="18" t="s">
         <v>138</v>
       </c>
       <c r="E30" s="2" t="s">
@@ -1999,16 +1999,16 @@
       <c r="B31" s="8">
         <v>6</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="19"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="21"/>
       <c r="K31" s="7"/>
     </row>
     <row r="32" spans="1:11" ht="90">
@@ -2078,16 +2078,16 @@
       <c r="B34" s="8">
         <v>7</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="21"/>
       <c r="K34" s="7"/>
     </row>
     <row r="35" spans="1:11" ht="72">
@@ -2188,16 +2188,16 @@
       <c r="B38" s="8">
         <v>8</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="19"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="21"/>
       <c r="K38" s="7"/>
     </row>
     <row r="39" spans="1:11" ht="90">
@@ -2277,6 +2277,7 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C38:J38"/>
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="C31:J31"/>
@@ -2284,7 +2285,6 @@
     <mergeCell ref="C34:J34"/>
     <mergeCell ref="C21:J21"/>
     <mergeCell ref="C8:J8"/>
-    <mergeCell ref="C38:J38"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Implemented C++ golden_model and integrated it with the system verilog golden_model
</commit_message>
<xml_diff>
--- a/verification plan/verification plan.xlsx
+++ b/verification plan/verification plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shared Folders\Uni\courses\Digital circuit\digital github codes\Done\spi\Verification-of-SPI-Slave-with-Single-Port-RAM\verification plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7B5C98-4FE1-4DB6-9B2A-556D3330C122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B682A3-4045-4B7F-B55C-854B0F19A4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BE33C207-AC50-49BB-BEDD-1F59C983F64D}"/>
   </bookViews>
@@ -1114,7 +1114,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>

</xml_diff>

<commit_message>
updated the run scripts
</commit_message>
<xml_diff>
--- a/verification plan/verification plan.xlsx
+++ b/verification plan/verification plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shared Folders\Uni\courses\Digital circuit\digital github codes\Done\spi\Verification-of-SPI-Slave-with-Single-Port-RAM\verification plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B682A3-4045-4B7F-B55C-854B0F19A4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C01C4F-AE56-4B00-8851-A2FB0088B34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BE33C207-AC50-49BB-BEDD-1F59C983F64D}"/>
   </bookViews>
@@ -1112,9 +1112,9 @@
   </sheetPr>
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>

</xml_diff>

<commit_message>
Successfully completed the verification of the RAM module, achieving 100% functional and code coverage.
</commit_message>
<xml_diff>
--- a/verification plan/verification plan.xlsx
+++ b/verification plan/verification plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shared Folders\Uni\courses\Digital circuit\digital github codes\Done\spi\Verification-of-SPI-Slave-with-Single-Port-RAM\verification plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C01C4F-AE56-4B00-8851-A2FB0088B34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F324BD-735A-4AA9-A044-B39EFB798289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BE33C207-AC50-49BB-BEDD-1F59C983F64D}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{BE33C207-AC50-49BB-BEDD-1F59C983F64D}"/>
   </bookViews>
   <sheets>
     <sheet name="Verification Plan" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="153">
   <si>
     <t>#</t>
   </si>
@@ -298,64 +298,25 @@
     <t>Verify that the RAM stores din[7:0] in the internal write address bus if din[9:8] == 2'b00</t>
   </si>
   <si>
-    <t>RAM internal signals checked against golden model.
-Concurrent assertion to check for the internal write address bus.</t>
-  </si>
-  <si>
     <t>RAM write data behaviour</t>
   </si>
   <si>
     <t>Verify that the RAM stores din[7:0] with write address previously held</t>
   </si>
   <si>
-    <t>RAM internal signals checked against golden model.
-Concurrent assertion to check for the writen data on RAM</t>
-  </si>
-  <si>
     <t>RAM read address behaviour</t>
   </si>
   <si>
     <t>Verify that the RAM stores din[7:0] in the internal read address bus</t>
   </si>
   <si>
-    <t>RAM internal signals checked against golden model.
-Concurrent assertion to check for the read data from RAM</t>
-  </si>
-  <si>
-    <t>RAM internal signals checked against golden model.
-Concurrent assertion to check for the read address at RAM</t>
-  </si>
-  <si>
     <t>RAM read data behaviour</t>
   </si>
   <si>
     <t>RAM Data is ready during rd_data control bits</t>
   </si>
   <si>
-    <t>Ensure that the RAM asserts tx_valid to inform slave that data out is ready</t>
-  </si>
-  <si>
     <t>Verify that the RAM will read from the memory with rd_address previously held</t>
-  </si>
-  <si>
-    <t>RAM internal signals checked against golden model.
-Concurrent assertion to check for the tx_valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constraint Randomization to randmoize the MOSI signal
-to allow only read data operations </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constraint Randomization to randmoize the MOSI signal
-to allow only read address operations  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constraint Randomization to randmoize the MOSI signal
-to allow only write data operations  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constraint Randomization to randmoize the MOSI signal
-to allow only write address operations  </t>
   </si>
   <si>
     <t>SPI Wrapper</t>
@@ -437,29 +398,6 @@
 </t>
   </si>
   <si>
-    <t>Assertion: assert_tx_valid
-Cross: TBA</t>
-  </si>
-  <si>
-    <t>Assertion: assert_rd_addr_ram
-Coverpoint: spi_cov_grp::data_out_cp
-Cross: TBA</t>
-  </si>
-  <si>
-    <t>Assertion: assert_rd_addr_ram
-Coverpoint: spi_cov_grp::addr_rd_cp
-Cross: TBA</t>
-  </si>
-  <si>
-    <t>Assertion: assert_wr_data_ram
-Cross: TBA</t>
-  </si>
-  <si>
-    <t>Assertion: assert_wr_addr_ram
-Coverpoint: spi_cov_grp::addr_wr_cp
-Cross: TBA</t>
-  </si>
-  <si>
     <t>Assertion: assert_read_add
 Cross: TBA</t>
   </si>
@@ -536,6 +474,77 @@
   </si>
   <si>
     <t>Constraint Randomization to randmoize the SS_n &amp; MOSI</t>
+  </si>
+  <si>
+    <t>Ensure that the RAM asserts tx_valid to inform slave that data out is ready and deasserts it otherwise</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constraint Randomization to randmoize the rx_valid and rx_data/din </t>
+  </si>
+  <si>
+    <t>Concurrent assertion to check for the internal write address bus.</t>
+  </si>
+  <si>
+    <t>RAM READ/WRITE</t>
+  </si>
+  <si>
+    <t>RAM Outputs</t>
+  </si>
+  <si>
+    <t>RAM output signals checked against golden model.</t>
+  </si>
+  <si>
+    <t>Ensure that the RAM supports both read and write operations by verifying its outputs against a golden reference model</t>
+  </si>
+  <si>
+    <t>Assertion: assert_rd_addr_ram
+Coverpoint: spi_cov_grp::addr_rd_cp
+Constraint Randomization: rx_valid_c
+Constraint Randomization: rx_data_c</t>
+  </si>
+  <si>
+    <t>Assertion: assert_rd_data_ram
+Coverpoint: spi_cov_grp::data_out_cp
+Constraint Randomization: rx_valid_c
+Constraint Randomization: rx_data_c</t>
+  </si>
+  <si>
+    <t>Assertion: assert_tx_valid
+Assertion: assert_rd_data_ram
+Constraint Randomization: rx_valid_c
+Constraint Randomization: rx_data_c</t>
+  </si>
+  <si>
+    <t>Assertion: assert_wr_data_ram
+Constraint Randomization: rx_valid_c
+Constraint Randomization: rx_data_c</t>
+  </si>
+  <si>
+    <t>Assertion: assert_wr_addr_ram
+Constraint Randomization: rx_valid_c
+Constraint Randomization: rx_data_c</t>
+  </si>
+  <si>
+    <t>Constraint Randomization: rx_valid_c
+Constraint Randomization: rx_data_c
+Coverpoint: spi_cov_grp::dout_cp
+Coverpoint: spi_cov_grp::tx_valid_cp
+Cross: spi_cov_grp::tx_valid_dout_cr</t>
+  </si>
+  <si>
+    <t>Concurrent assertion to check for the internal read address of the RAM</t>
+  </si>
+  <si>
+    <t>Concurrent assertion to check for the dout &amp; tx_valid of the RAM</t>
+  </si>
+  <si>
+    <t>Concurrent assertion to check for the tx_valid of the RAM</t>
+  </si>
+  <si>
+    <t>Concurrent assertion to check for the writen data on the internal array mem of the RAM</t>
   </si>
 </sst>
 </file>
@@ -758,13 +767,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1110,11 +1119,11 @@
     <tabColor theme="3" tint="0.249977111117893"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1187,13 +1196,13 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>79</v>
@@ -1249,13 +1258,13 @@
         <v>1.3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>79</v>
@@ -1352,10 +1361,10 @@
         <v>19</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>55</v>
@@ -1386,7 +1395,7 @@
         <v>32</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>56</v>
@@ -1414,10 +1423,10 @@
         <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>57</v>
@@ -1445,10 +1454,10 @@
         <v>21</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>58</v>
@@ -1476,10 +1485,10 @@
         <v>35</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>59</v>
@@ -1507,10 +1516,10 @@
         <v>37</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>60</v>
@@ -1538,10 +1547,10 @@
         <v>38</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>61</v>
@@ -1569,10 +1578,10 @@
         <v>66</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>61</v>
@@ -1600,10 +1609,10 @@
         <v>40</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>62</v>
@@ -1631,10 +1640,10 @@
         <v>68</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>69</v>
@@ -1662,10 +1671,10 @@
         <v>23</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>63</v>
@@ -1693,10 +1702,10 @@
         <v>27</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>64</v>
@@ -1772,7 +1781,7 @@
         <v>71</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>73</v>
@@ -1803,7 +1812,7 @@
         <v>72</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>73</v>
@@ -1834,7 +1843,7 @@
         <v>73</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>73</v>
@@ -1865,7 +1874,7 @@
         <v>73</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>73</v>
@@ -1890,7 +1899,7 @@
         <v>5</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
@@ -1907,16 +1916,16 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>80</v>
@@ -1938,16 +1947,16 @@
         <v>5.2</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>82</v>
@@ -1969,19 +1978,19 @@
         <v>5.3</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="H30" s="1">
         <v>1</v>
@@ -2000,7 +2009,7 @@
         <v>6</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
@@ -2011,7 +2020,7 @@
       <c r="J31" s="21"/>
       <c r="K31" s="7"/>
     </row>
-    <row r="32" spans="1:11" ht="90">
+    <row r="32" spans="1:11" ht="54">
       <c r="A32" s="10"/>
       <c r="B32" s="1">
         <v>6.1</v>
@@ -2023,13 +2032,13 @@
         <v>84</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>101</v>
+        <v>137</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>85</v>
+        <v>138</v>
       </c>
       <c r="H32" s="1">
         <v>1</v>
@@ -2038,29 +2047,29 @@
         <v>100</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" ht="72">
+    <row r="33" spans="1:11" ht="54">
       <c r="A33" s="10"/>
       <c r="B33" s="1">
         <v>6.2</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>100</v>
+        <v>137</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
       <c r="H33" s="1">
         <v>1</v>
@@ -2069,7 +2078,7 @@
         <v>100</v>
       </c>
       <c r="J33" s="12" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="K33" s="7"/>
     </row>
@@ -2079,7 +2088,7 @@
         <v>7</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
@@ -2096,19 +2105,19 @@
         <v>7.1</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>92</v>
+        <v>149</v>
       </c>
       <c r="H35" s="1">
         <v>1</v>
@@ -2117,7 +2126,7 @@
         <v>100</v>
       </c>
       <c r="J35" s="12" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="K35" s="7"/>
     </row>
@@ -2127,19 +2136,19 @@
         <v>7.2</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>91</v>
+        <v>150</v>
       </c>
       <c r="H36" s="1">
         <v>1</v>
@@ -2148,7 +2157,7 @@
         <v>100</v>
       </c>
       <c r="J36" s="12" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="K36" s="7"/>
     </row>
@@ -2158,19 +2167,19 @@
         <v>7.3</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
       <c r="H37" s="1">
         <v>1</v>
@@ -2179,7 +2188,7 @@
         <v>100</v>
       </c>
       <c r="J37" s="12" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="K37" s="7"/>
     </row>
@@ -2189,7 +2198,7 @@
         <v>8</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>102</v>
+        <v>139</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
@@ -2206,19 +2215,19 @@
         <v>8.1</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>106</v>
+        <v>142</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>103</v>
+        <v>148</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="H39" s="1">
         <v>1</v>
@@ -2226,58 +2235,106 @@
       <c r="I39" s="2">
         <v>100</v>
       </c>
-      <c r="J39" s="12" t="s">
-        <v>12</v>
+      <c r="J39" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:11" ht="54">
+    <row r="40" spans="1:11" ht="21.75">
       <c r="A40" s="10"/>
-      <c r="B40" s="1">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H40" s="1">
-        <v>1</v>
-      </c>
-      <c r="I40" s="2">
-        <v>100</v>
-      </c>
-      <c r="J40" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="B40" s="8">
+        <v>9</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="21"/>
       <c r="K40" s="7"/>
     </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
+    <row r="41" spans="1:11" ht="90">
+      <c r="A41" s="10"/>
+      <c r="B41" s="1">
+        <v>9.1</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H41" s="1">
+        <v>1</v>
+      </c>
+      <c r="I41" s="2">
+        <v>100</v>
+      </c>
+      <c r="J41" s="12" t="s">
+        <v>12</v>
+      </c>
       <c r="K41" s="7"/>
     </row>
+    <row r="42" spans="1:11" ht="54">
+      <c r="A42" s="10"/>
+      <c r="B42" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H42" s="1">
+        <v>1</v>
+      </c>
+      <c r="I42" s="2">
+        <v>100</v>
+      </c>
+      <c r="J42" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K42" s="7"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="C38:J38"/>
+  <mergeCells count="9">
+    <mergeCell ref="C40:J40"/>
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="C31:J31"/>
@@ -2285,6 +2342,7 @@
     <mergeCell ref="C34:J34"/>
     <mergeCell ref="C21:J21"/>
     <mergeCell ref="C8:J8"/>
+    <mergeCell ref="C38:J38"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>